<commit_message>
Sensitive API changes for Entity APIs
</commit_message>
<xml_diff>
--- a/_apidocs/entity-api/v1/entity-sample-csv.xlsx
+++ b/_apidocs/entity-api/v1/entity-sample-csv.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\open-gsa-redesign\_apidocs\entity-api\v1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC83805-AF82-4E58-BA78-FD513AB4943A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="350" windowWidth="18660" windowHeight="7060"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entity-CSV" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="482">
   <si>
     <t>ueiSAM</t>
   </si>
@@ -1457,12 +1463,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1984,6 +1993,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2031,7 +2043,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2064,9 +2076,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2099,6 +2128,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2274,136 +2320,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:PM8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BQ8" sqref="BQ8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" customWidth="1"/>
-    <col min="4" max="11" width="9.23046875" customWidth="1"/>
-    <col min="12" max="12" width="13.921875" customWidth="1"/>
-    <col min="13" max="13" width="13.69140625" customWidth="1"/>
-    <col min="14" max="14" width="22.23046875" customWidth="1"/>
-    <col min="15" max="16" width="12.3828125" customWidth="1"/>
-    <col min="17" max="17" width="15.3828125" customWidth="1"/>
-    <col min="18" max="18" width="14.15234375" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
+    <col min="4" max="11" width="9.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" customWidth="1"/>
+    <col min="14" max="14" width="22.26953125" customWidth="1"/>
+    <col min="15" max="16" width="12.36328125" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" customWidth="1"/>
+    <col min="18" max="18" width="14.1796875" customWidth="1"/>
     <col min="19" max="19" width="18" customWidth="1"/>
-    <col min="20" max="20" width="17.69140625" customWidth="1"/>
-    <col min="21" max="22" width="12.15234375" customWidth="1"/>
-    <col min="23" max="23" width="26.61328125" customWidth="1"/>
-    <col min="24" max="24" width="27.921875" customWidth="1"/>
-    <col min="25" max="25" width="36.84375" customWidth="1"/>
+    <col min="20" max="20" width="17.7265625" customWidth="1"/>
+    <col min="21" max="22" width="12.1796875" customWidth="1"/>
+    <col min="23" max="23" width="26.6328125" customWidth="1"/>
+    <col min="24" max="24" width="27.90625" customWidth="1"/>
+    <col min="25" max="25" width="36.81640625" customWidth="1"/>
     <col min="26" max="26" width="34" customWidth="1"/>
-    <col min="27" max="27" width="32.23046875" customWidth="1"/>
-    <col min="28" max="28" width="20.69140625" customWidth="1"/>
-    <col min="29" max="29" width="22.07421875" customWidth="1"/>
+    <col min="27" max="27" width="32.26953125" customWidth="1"/>
+    <col min="28" max="28" width="20.7265625" customWidth="1"/>
+    <col min="29" max="29" width="22.08984375" customWidth="1"/>
     <col min="30" max="30" width="31" customWidth="1"/>
-    <col min="31" max="32" width="25.61328125" customWidth="1"/>
-    <col min="33" max="33" width="17.15234375" customWidth="1"/>
-    <col min="34" max="34" width="32.15234375" customWidth="1"/>
+    <col min="31" max="32" width="25.6328125" customWidth="1"/>
+    <col min="33" max="33" width="17.1796875" customWidth="1"/>
+    <col min="34" max="34" width="32.1796875" customWidth="1"/>
     <col min="35" max="35" width="25" customWidth="1"/>
-    <col min="36" max="36" width="21.23046875" customWidth="1"/>
+    <col min="36" max="36" width="21.26953125" customWidth="1"/>
     <col min="37" max="37" width="26" customWidth="1"/>
-    <col min="38" max="38" width="26.3828125" customWidth="1"/>
-    <col min="39" max="39" width="19.921875" customWidth="1"/>
-    <col min="40" max="40" width="16.69140625" customWidth="1"/>
-    <col min="41" max="41" width="34.53515625" customWidth="1"/>
-    <col min="42" max="43" width="20.23046875" customWidth="1"/>
-    <col min="44" max="44" width="11.765625" customWidth="1"/>
-    <col min="45" max="45" width="26.84375" customWidth="1"/>
-    <col min="46" max="46" width="19.69140625" customWidth="1"/>
-    <col min="47" max="47" width="15.84375" customWidth="1"/>
-    <col min="48" max="48" width="20.61328125" customWidth="1"/>
-    <col min="49" max="49" width="21.07421875" customWidth="1"/>
-    <col min="50" max="50" width="24.61328125" customWidth="1"/>
-    <col min="51" max="58" width="9.23046875" customWidth="1"/>
-    <col min="59" max="59" width="29.921875" customWidth="1"/>
-    <col min="60" max="60" width="30.3046875" customWidth="1"/>
+    <col min="38" max="38" width="26.36328125" customWidth="1"/>
+    <col min="39" max="39" width="19.90625" customWidth="1"/>
+    <col min="40" max="40" width="16.7265625" customWidth="1"/>
+    <col min="41" max="41" width="34.54296875" customWidth="1"/>
+    <col min="42" max="43" width="20.26953125" customWidth="1"/>
+    <col min="44" max="44" width="11.7265625" customWidth="1"/>
+    <col min="45" max="45" width="26.81640625" customWidth="1"/>
+    <col min="46" max="46" width="19.7265625" customWidth="1"/>
+    <col min="47" max="47" width="15.81640625" customWidth="1"/>
+    <col min="48" max="48" width="20.6328125" customWidth="1"/>
+    <col min="49" max="49" width="21.08984375" customWidth="1"/>
+    <col min="50" max="50" width="24.6328125" customWidth="1"/>
+    <col min="51" max="58" width="9.26953125" customWidth="1"/>
+    <col min="59" max="59" width="29.90625" customWidth="1"/>
+    <col min="60" max="60" width="30.26953125" customWidth="1"/>
     <col min="61" max="61" width="30" customWidth="1"/>
-    <col min="62" max="62" width="21.4609375" customWidth="1"/>
-    <col min="63" max="63" width="29.4609375" customWidth="1"/>
-    <col min="64" max="64" width="27.53515625" customWidth="1"/>
+    <col min="62" max="62" width="21.453125" customWidth="1"/>
+    <col min="63" max="63" width="29.453125" customWidth="1"/>
+    <col min="64" max="64" width="27.54296875" customWidth="1"/>
     <col min="65" max="65" width="23" customWidth="1"/>
-    <col min="66" max="67" width="24.07421875" customWidth="1"/>
-    <col min="68" max="68" width="15.61328125" customWidth="1"/>
-    <col min="69" max="69" width="19.69140625" customWidth="1"/>
-    <col min="70" max="70" width="24.4609375" customWidth="1"/>
-    <col min="71" max="71" width="30.69140625" customWidth="1"/>
-    <col min="72" max="72" width="23.53515625" customWidth="1"/>
-    <col min="73" max="73" width="6.4609375" customWidth="1"/>
-    <col min="74" max="74" width="22.765625" customWidth="1"/>
-    <col min="75" max="81" width="9.23046875" customWidth="1"/>
-    <col min="82" max="82" width="13.15234375" customWidth="1"/>
-    <col min="83" max="83" width="21.07421875" customWidth="1"/>
-    <col min="84" max="84" width="19.921875" customWidth="1"/>
-    <col min="85" max="85" width="26.3046875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="32.84375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="21.921875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="26.69140625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="25.765625" bestFit="1" customWidth="1"/>
-    <col min="92" max="93" width="25.4609375" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="24.08984375" customWidth="1"/>
+    <col min="68" max="68" width="15.6328125" customWidth="1"/>
+    <col min="69" max="69" width="19.7265625" customWidth="1"/>
+    <col min="70" max="70" width="24.453125" customWidth="1"/>
+    <col min="71" max="71" width="30.7265625" customWidth="1"/>
+    <col min="72" max="72" width="23.54296875" customWidth="1"/>
+    <col min="73" max="73" width="6.453125" customWidth="1"/>
+    <col min="74" max="74" width="22.7265625" customWidth="1"/>
+    <col min="75" max="81" width="9.26953125" customWidth="1"/>
+    <col min="82" max="82" width="13.1796875" customWidth="1"/>
+    <col min="83" max="83" width="21.08984375" customWidth="1"/>
+    <col min="84" max="84" width="19.90625" customWidth="1"/>
+    <col min="85" max="85" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="17" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="32" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="21.07421875" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="24.84375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="26" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="25.765625" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="19.921875" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="19.921875" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="36.84375" style="2" customWidth="1"/>
-    <col min="133" max="133" width="24.3828125" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="30.61328125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="25.4609375" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="16.765625" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="16.3046875" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="12.921875" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="13.07421875" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="21.4609375" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="19.921875" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="30.921875" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="32.921875" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="30.4609375" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="27.3828125" bestFit="1" customWidth="1"/>
-    <col min="252" max="253" width="34.23046875" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="25.765625" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="29.84375" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="34.61328125" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="33.69140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="36.81640625" style="2" customWidth="1"/>
+    <col min="133" max="133" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="252" max="253" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="33.7265625" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="29" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="28.921875" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="28.53515625" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="268" max="269" width="32.3046875" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="23.84375" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="27.921875" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="31.765625" bestFit="1" customWidth="1"/>
-    <col min="364" max="364" width="30.07421875" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="268" max="269" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="364" max="364" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="367" max="367" width="25" bestFit="1" customWidth="1"/>
-    <col min="368" max="368" width="29.61328125" bestFit="1" customWidth="1"/>
-    <col min="369" max="369" width="37.84375" bestFit="1" customWidth="1"/>
-    <col min="370" max="370" width="33.3828125" bestFit="1" customWidth="1"/>
-    <col min="371" max="371" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="372" max="372" width="26.53515625" bestFit="1" customWidth="1"/>
-    <col min="389" max="389" width="15.765625" bestFit="1" customWidth="1"/>
-    <col min="391" max="391" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="393" max="393" width="15.3046875" bestFit="1" customWidth="1"/>
-    <col min="394" max="394" width="23.53515625" bestFit="1" customWidth="1"/>
-    <col min="395" max="395" width="19.07421875" bestFit="1" customWidth="1"/>
-    <col min="396" max="396" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="397" max="397" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="368" max="368" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="369" max="369" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="370" max="370" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="371" max="371" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="372" max="372" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="389" max="389" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="391" max="391" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="393" max="393" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="394" max="394" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="395" max="395" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="396" max="396" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="397" max="397" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:429" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>446</v>
       </c>
@@ -3692,9 +3738,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:429" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:429" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
       <c r="B2" t="s">
         <v>447</v>
@@ -3757,7 +3803,7 @@
         <v>412</v>
       </c>
       <c r="V2" t="s">
-        <v>420</v>
+        <v>481</v>
       </c>
       <c r="W2" t="s">
         <v>447</v>
@@ -4975,7 +5021,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:429" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
       <c r="L8" s="2"/>
       <c r="S8" s="2"/>
     </row>

</xml_diff>